<commit_message>
no more data spreadsheets
</commit_message>
<xml_diff>
--- a/data/2023-12-10.xlsx
+++ b/data/2023-12-10.xlsx
@@ -8,6 +8,17 @@
   <sheets>
     <sheet name="1000" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="1200" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="1300" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="1400" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="1500" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="1600" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="1700" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="1800" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="1900" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="2000" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="2100" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="2200" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="2300" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -944,6 +955,598 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>I Love You So</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>The Walters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>I Love You So</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>160.239</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2014-11-28</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:59:33.227Z</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>The Sunshine</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Manchester Orchestra</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>A Black Mile To The Surface</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>117.173</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2017-07-28</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:56:52.273Z</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Your Dog</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Soccer Mommy</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Clean</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>194.009</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2018-03-02</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:54:55.293Z</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Harvey</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Her's</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Invitation to Her's</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>211.165</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2018-08-24</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:51:40.222Z</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Marcel</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Her's</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Songs of Her's</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>187.571</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2017-05-12</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:48:08.812Z</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Alrighty Aphrodite</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Peach Pit</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Being So Normal</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>207.813</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2018-06-28</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:45:01.008Z</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Motion Sickness</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Phoebe Bridgers</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Stranger in the Alps</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>229.76</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2017-09-22</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:41:32.088Z</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Another One</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mac DeMarco</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Another One</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>160.991</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2015-08-07</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:37:42.295Z</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Blue Boy</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mac DeMarco</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Salad Days</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>126.223</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2014-04-01</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:35:00.594Z</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Vacations</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Vibes</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>145.666</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2023-12-10T21:32:54.263Z</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Sports</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Beach Bunny</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Sports</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>164.165</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2018-01-01</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2023-12-10T22:08:47.438Z</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Still Woozy</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>142.5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2018-03-22</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-12-10T22:06:02.829Z</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>4am</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>girl in red</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4am</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>110.861</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2018-08-10</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-12-10T22:03:39.804Z</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sweet Pill</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Where the Heart Is</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>134.972</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2022-05-25</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2023-12-10T22:01:49.329Z</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1590,4 +2193,947 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>EdEddnEddy</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>JID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>The Never Story</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>140.511</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2017-03-10</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2023-12-10T12:24:47.749Z</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Near</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bilmuri</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Letters</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>128.869</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2016-11-21</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-12-10T12:22:34.957Z</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>lvl99ROIDMAGE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bilmuri</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>400LB BACK SQUAT</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>201.658</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2021-09-27</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-12-10T12:20:27.926Z</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>spacesbetweenlettersarecool</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bilmuri</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>wet milk</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>158.374</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2019-04-19</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2023-12-10T12:17:29.415Z</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LIVIN' LAUGHIN' LOVIN'</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bilmuri</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>LIVIN' LAUGHIN' LOVIN'</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>166.959</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2023-06-23</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2023-12-10T12:15:10.227Z</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CORN-FED YETIS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bilmuri</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>GOBLIN HOURS</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>188.638</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2022-10-14</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2023-12-10T12:04:28.092Z</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Evergreen</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Richy Mitch &amp; The Coal Miners</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>RMCM</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>87.0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2017-05-17</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2023-12-10T12:01:17.489Z</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>EARFQUAKE</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tyler, The Creator</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>IGOR</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>190.066</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2019-05-17</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2023-12-10T13:13:15.743Z</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>IV. Sweatpants</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Childish Gambino</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Because the Internet</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>180.675</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2013-12-10</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-12-10T13:10:04.739Z</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Cooks</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Still Woozy</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cooks</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>174.105</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2017-07-16</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:58:06.375Z</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>British</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Dino Gala</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>British</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>135.957</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2022-02-18</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:55:12.107Z</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Fill in the Blank</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car Seat Headrest</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Teens Of Denial</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>244.506</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2016-05-20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:52:55.637Z</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Don't Think It Over</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Her's</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Invitation to Her's</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>246.362</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2018-08-24</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:48:50.316Z</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sweet Talk</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Dear and the Headlights</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Small Steps, Heavy Hooves</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>177.066</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2007</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:44:44.301Z</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Still Beating</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mac DeMarco</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>This Old Dog</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>181.586</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2017-05-05</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:41:45.834Z</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Weeds</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Beach Bunny</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Emotional Creature</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>202.693</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2022-07-22</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:38:43.947Z</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Speed Racer</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Her's</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Songs of Her's</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>151.722</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2017-05-12</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:35:21.474Z</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>She Needs Him</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Her's</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Invitation to Her's</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>314.39</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2018-08-24</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:30:12.532Z</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Dorothy</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Her's</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Songs of Her's</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>246.23</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2017-05-12</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:24:57.685Z</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>boys beware</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mad Tsai</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>boys beware</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>133.887</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-11-10</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:19:15.721Z</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sweater Weather</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>The Neighbourhood</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>I Love You.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>240.4</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2013-04-19</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:17:01.767Z</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BATTER UP</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BABYMONSTER</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BABYMONSTER Debut Digital Single [BATTER UP]</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>188.179</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-12-10T17:13:21.525Z</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>